<commit_message>
add poetry to repo
</commit_message>
<xml_diff>
--- a/kakao_developers/building_locations.xlsx
+++ b/kakao_developers/building_locations.xlsx
@@ -444,11 +444,15 @@
           <t>국립중앙박물관</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>37.52384681210344</v>
-      </c>
-      <c r="C2" t="n">
-        <v>126.9802030188691</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>37.523846812103436</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>126.98020301886912</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -457,11 +461,15 @@
           <t>서울시청</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>37.56682420267543</v>
-      </c>
-      <c r="C3" t="n">
-        <v>126.978652258823</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>37.56682420267543</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>126.978652258823</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -470,11 +478,15 @@
           <t>롯데월드타워</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>37.51260447840551</v>
-      </c>
-      <c r="C4" t="n">
-        <v>127.1025555865833</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>37.51260447840551</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>127.10255558658325</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>